<commit_message>
fix bug in formatting for nil cells, update tests to work for latest features
</commit_message>
<xml_diff>
--- a/spec/support/static_test_files/horizontal_and_vertical_alignment.xlsx
+++ b/spec/support/static_test_files/horizontal_and_vertical_alignment.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23515"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11208"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/f3m-mbp1/dev/f3mmedia/rxl/spec/support/static_test_files/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2D7B2DE-FCAC-8D44-B4C6-6D2D9B9A2862}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="16060" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="values" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="1">
   <si>
     <t>abc</t>
   </si>
@@ -27,7 +33,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -77,7 +83,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -106,6 +112,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -116,6 +129,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -440,16 +461,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -459,8 +480,12 @@
       <c r="C1" s="7" t="s">
         <v>0</v>
       </c>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10" t="s">
+        <v>0</v>
+      </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
@@ -470,8 +495,12 @@
       <c r="C2" s="9" t="s">
         <v>0</v>
       </c>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11" t="s">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -481,9 +510,8 @@
       <c r="C3" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
+      <c r="D3" s="12"/>
+      <c r="E3" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>